<commit_message>
Finally completed the buy from any excel file, also logging when products of that type aren't found
</commit_message>
<xml_diff>
--- a/Files/PO.xlsx
+++ b/Files/PO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stupa\OneDrive\Documents\UiPath\Development_DemoBlaze\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0BF7840-8901-4ED3-9451-633B7C6C018C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69DCC2DD-1C46-43E1-A0CD-47BA869679E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4236" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{44CE57F5-DC85-4DDB-95A4-CF63505EB0BD}"/>
+    <workbookView xWindow="4920" yWindow="3288" windowWidth="17280" windowHeight="8880" xr2:uid="{44CE57F5-DC85-4DDB-95A4-CF63505EB0BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Category</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>Logitech</t>
+  </si>
+  <si>
+    <t>Samsung</t>
   </si>
 </sst>
 </file>
@@ -433,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D35C9475-86DE-4DC6-9067-7858CC25C766}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -470,7 +473,7 @@
         <v>6</v>
       </c>
       <c r="C2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D2">
         <v>500</v>
@@ -521,10 +524,10 @@
         <v>11</v>
       </c>
       <c r="C5">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="E5">
         <v>500</v>
@@ -549,18 +552,52 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>231</v>
+      </c>
+      <c r="E7">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>500</v>
+      </c>
+      <c r="E8">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B9" t="s">
         <v>14</v>
       </c>
-      <c r="C7">
+      <c r="C9">
         <v>3</v>
       </c>
-      <c r="D7">
+      <c r="D9">
         <v>100</v>
       </c>
-      <c r="E7">
+      <c r="E9">
         <v>200</v>
       </c>
     </row>

</xml_diff>